<commit_message>
Changes to Main Form, ReportFormat2.xlsx and the Format 2 Report
</commit_message>
<xml_diff>
--- a/Impilo App/Templates/ReportFormat2.xlsx
+++ b/Impilo App/Templates/ReportFormat2.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -587,7 +587,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="33">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -811,12 +811,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -1382,7 +1376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="186">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1597,9 +1591,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1675,17 +1666,8 @@
     <xf numFmtId="0" fontId="28" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="28" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1714,101 +1696,77 @@
     <xf numFmtId="0" fontId="27" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1816,6 +1774,75 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1828,80 +1855,11 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="10" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2262,14 +2220,14 @@
       <c r="W9" s="28"/>
     </row>
     <row r="10" spans="1:23" s="3" customFormat="1" ht="98.25" customHeight="1">
-      <c r="A10" s="101"/>
-      <c r="B10" s="98" t="s">
+      <c r="A10" s="100"/>
+      <c r="B10" s="97" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="157" t="s">
+      <c r="C10" s="168" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="157"/>
+      <c r="D10" s="168"/>
       <c r="E10" s="26" t="s">
         <v>13</v>
       </c>
@@ -2285,31 +2243,31 @@
       <c r="I10" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="J10" s="151" t="s">
+      <c r="J10" s="173" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="151"/>
+      <c r="K10" s="173"/>
       <c r="L10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M10" s="151" t="s">
+      <c r="M10" s="173" t="s">
         <v>17</v>
       </c>
-      <c r="N10" s="151"/>
-      <c r="O10" s="151"/>
-      <c r="P10" s="151"/>
-      <c r="Q10" s="151" t="s">
+      <c r="N10" s="173"/>
+      <c r="O10" s="173"/>
+      <c r="P10" s="173"/>
+      <c r="Q10" s="173" t="s">
         <v>18</v>
       </c>
-      <c r="R10" s="151"/>
-      <c r="S10" s="151" t="s">
+      <c r="R10" s="173"/>
+      <c r="S10" s="173" t="s">
         <v>19</v>
       </c>
-      <c r="T10" s="151"/>
-      <c r="U10" s="151" t="s">
+      <c r="T10" s="173"/>
+      <c r="U10" s="173" t="s">
         <v>20</v>
       </c>
-      <c r="V10" s="151"/>
+      <c r="V10" s="173"/>
       <c r="W10" s="1" t="s">
         <v>21</v>
       </c>
@@ -2318,65 +2276,65 @@
       <c r="A11" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="102"/>
-      <c r="C11" s="99" t="s">
+      <c r="B11" s="101"/>
+      <c r="C11" s="98" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="104"/>
-      <c r="E11" s="105"/>
-      <c r="F11" s="105"/>
-      <c r="G11" s="105"/>
-      <c r="H11" s="105"/>
-      <c r="I11" s="105"/>
-      <c r="J11" s="106"/>
-      <c r="K11" s="106"/>
-      <c r="L11" s="105"/>
-      <c r="M11" s="105"/>
+      <c r="D11" s="103"/>
+      <c r="E11" s="104"/>
+      <c r="F11" s="104"/>
+      <c r="G11" s="104"/>
+      <c r="H11" s="104"/>
+      <c r="I11" s="104"/>
+      <c r="J11" s="105"/>
+      <c r="K11" s="105"/>
+      <c r="L11" s="104"/>
+      <c r="M11" s="104"/>
       <c r="N11" s="27"/>
       <c r="O11" s="27"/>
       <c r="P11" s="27"/>
-      <c r="Q11" s="105"/>
-      <c r="R11" s="112"/>
-      <c r="S11" s="105"/>
-      <c r="T11" s="112"/>
-      <c r="U11" s="105"/>
-      <c r="V11" s="112"/>
-      <c r="W11" s="105"/>
+      <c r="Q11" s="104"/>
+      <c r="R11" s="109"/>
+      <c r="S11" s="104"/>
+      <c r="T11" s="109"/>
+      <c r="U11" s="104"/>
+      <c r="V11" s="109"/>
+      <c r="W11" s="104"/>
     </row>
     <row r="12" spans="1:23" s="3" customFormat="1" ht="91.5" customHeight="1" thickBot="1">
       <c r="A12" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="103"/>
+      <c r="B12" s="102"/>
       <c r="C12" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="107"/>
-      <c r="E12" s="108"/>
-      <c r="F12" s="108"/>
-      <c r="G12" s="108"/>
-      <c r="H12" s="108"/>
-      <c r="I12" s="108"/>
-      <c r="J12" s="108"/>
-      <c r="K12" s="109"/>
-      <c r="L12" s="108"/>
-      <c r="M12" s="108"/>
+      <c r="D12" s="106"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="107"/>
+      <c r="G12" s="107"/>
+      <c r="H12" s="107"/>
+      <c r="I12" s="107"/>
+      <c r="J12" s="107"/>
+      <c r="K12" s="108"/>
+      <c r="L12" s="107"/>
+      <c r="M12" s="107"/>
       <c r="N12" s="27"/>
       <c r="O12" s="27"/>
       <c r="P12" s="27"/>
-      <c r="Q12" s="108"/>
-      <c r="R12" s="112"/>
-      <c r="S12" s="108"/>
-      <c r="T12" s="112"/>
-      <c r="U12" s="108"/>
-      <c r="V12" s="112"/>
-      <c r="W12" s="108"/>
+      <c r="Q12" s="107"/>
+      <c r="R12" s="109"/>
+      <c r="S12" s="107"/>
+      <c r="T12" s="109"/>
+      <c r="U12" s="107"/>
+      <c r="V12" s="109"/>
+      <c r="W12" s="107"/>
     </row>
     <row r="13" spans="1:23" s="5" customFormat="1" ht="38.25">
       <c r="A13" s="4"/>
       <c r="B13" s="46"/>
-      <c r="C13" s="158"/>
-      <c r="D13" s="159"/>
+      <c r="C13" s="169"/>
+      <c r="D13" s="170"/>
       <c r="E13" s="47"/>
       <c r="F13" s="47"/>
       <c r="G13" s="47"/>
@@ -2424,8 +2382,8 @@
     <row r="14" spans="1:23" s="18" customFormat="1" ht="102.75" customHeight="1">
       <c r="A14" s="4"/>
       <c r="B14" s="29"/>
-      <c r="C14" s="153"/>
-      <c r="D14" s="154"/>
+      <c r="C14" s="166"/>
+      <c r="D14" s="167"/>
       <c r="E14" s="29"/>
       <c r="F14" s="29"/>
       <c r="G14" s="29"/>
@@ -2434,23 +2392,23 @@
       <c r="J14" s="29"/>
       <c r="K14" s="29"/>
       <c r="L14" s="29"/>
-      <c r="M14" s="105"/>
-      <c r="N14" s="105"/>
-      <c r="O14" s="105"/>
-      <c r="P14" s="105"/>
-      <c r="Q14" s="105"/>
-      <c r="R14" s="105"/>
-      <c r="S14" s="105"/>
-      <c r="T14" s="105"/>
-      <c r="U14" s="105"/>
-      <c r="V14" s="105"/>
+      <c r="M14" s="104"/>
+      <c r="N14" s="104"/>
+      <c r="O14" s="104"/>
+      <c r="P14" s="104"/>
+      <c r="Q14" s="104"/>
+      <c r="R14" s="104"/>
+      <c r="S14" s="104"/>
+      <c r="T14" s="104"/>
+      <c r="U14" s="104"/>
+      <c r="V14" s="104"/>
       <c r="W14" s="32"/>
     </row>
     <row r="15" spans="1:23" s="18" customFormat="1" ht="123" customHeight="1">
       <c r="A15" s="4"/>
       <c r="B15" s="29"/>
-      <c r="C15" s="153"/>
-      <c r="D15" s="154"/>
+      <c r="C15" s="166"/>
+      <c r="D15" s="167"/>
       <c r="E15" s="30"/>
       <c r="F15" s="30"/>
       <c r="G15" s="30"/>
@@ -2459,16 +2417,16 @@
       <c r="J15" s="27"/>
       <c r="K15" s="27"/>
       <c r="L15" s="30"/>
-      <c r="M15" s="115"/>
-      <c r="N15" s="115"/>
-      <c r="O15" s="115"/>
-      <c r="P15" s="115"/>
-      <c r="Q15" s="115"/>
-      <c r="R15" s="115"/>
-      <c r="S15" s="115"/>
-      <c r="T15" s="115"/>
-      <c r="U15" s="115"/>
-      <c r="V15" s="115"/>
+      <c r="M15" s="111"/>
+      <c r="N15" s="111"/>
+      <c r="O15" s="111"/>
+      <c r="P15" s="111"/>
+      <c r="Q15" s="111"/>
+      <c r="R15" s="111"/>
+      <c r="S15" s="111"/>
+      <c r="T15" s="111"/>
+      <c r="U15" s="111"/>
+      <c r="V15" s="111"/>
       <c r="W15" s="32"/>
     </row>
     <row r="16" spans="1:23" s="21" customFormat="1">
@@ -2496,10 +2454,10 @@
     <row r="17" spans="1:23" ht="76.5">
       <c r="A17" s="6"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="160" t="s">
+      <c r="C17" s="171" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="160"/>
+      <c r="D17" s="171"/>
       <c r="E17" s="7" t="s">
         <v>27</v>
       </c>
@@ -2514,91 +2472,91 @@
       <c r="L17" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="M17" s="150" t="s">
+      <c r="M17" s="172" t="s">
         <v>30</v>
       </c>
-      <c r="N17" s="150"/>
-      <c r="O17" s="150"/>
-      <c r="P17" s="150"/>
-      <c r="Q17" s="150" t="s">
+      <c r="N17" s="172"/>
+      <c r="O17" s="172"/>
+      <c r="P17" s="172"/>
+      <c r="Q17" s="172" t="s">
         <v>31</v>
       </c>
-      <c r="R17" s="150"/>
-      <c r="S17" s="150" t="s">
+      <c r="R17" s="172"/>
+      <c r="S17" s="172" t="s">
         <v>32</v>
       </c>
-      <c r="T17" s="150"/>
-      <c r="U17" s="150" t="s">
+      <c r="T17" s="172"/>
+      <c r="U17" s="172" t="s">
         <v>33</v>
       </c>
-      <c r="V17" s="150"/>
+      <c r="V17" s="172"/>
       <c r="W17" s="31" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="88.5" customHeight="1" thickBot="1">
-      <c r="A18" s="87" t="s">
+      <c r="A18" s="86" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="116"/>
-      <c r="E18" s="105"/>
-      <c r="F18" s="117"/>
-      <c r="G18" s="117"/>
-      <c r="H18" s="105"/>
-      <c r="I18" s="117"/>
-      <c r="J18" s="117"/>
-      <c r="K18" s="117"/>
-      <c r="L18" s="105"/>
-      <c r="M18" s="105"/>
-      <c r="N18" s="118"/>
-      <c r="O18" s="118"/>
-      <c r="P18" s="118"/>
-      <c r="Q18" s="105"/>
-      <c r="R18" s="118"/>
-      <c r="S18" s="105"/>
-      <c r="T18" s="117"/>
-      <c r="U18" s="105"/>
-      <c r="V18" s="117"/>
-      <c r="W18" s="105"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="113"/>
+      <c r="G18" s="113"/>
+      <c r="H18" s="104"/>
+      <c r="I18" s="113"/>
+      <c r="J18" s="113"/>
+      <c r="K18" s="113"/>
+      <c r="L18" s="104"/>
+      <c r="M18" s="104"/>
+      <c r="N18" s="114"/>
+      <c r="O18" s="114"/>
+      <c r="P18" s="114"/>
+      <c r="Q18" s="104"/>
+      <c r="R18" s="114"/>
+      <c r="S18" s="104"/>
+      <c r="T18" s="113"/>
+      <c r="U18" s="104"/>
+      <c r="V18" s="113"/>
+      <c r="W18" s="104"/>
     </row>
     <row r="19" spans="1:23" ht="81" customHeight="1" thickBot="1">
-      <c r="A19" s="88" t="s">
+      <c r="A19" s="87" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="119"/>
-      <c r="E19" s="108"/>
-      <c r="F19" s="120"/>
-      <c r="G19" s="120"/>
-      <c r="H19" s="108"/>
-      <c r="I19" s="120"/>
-      <c r="J19" s="120"/>
-      <c r="K19" s="120"/>
-      <c r="L19" s="108"/>
-      <c r="M19" s="108"/>
-      <c r="N19" s="121"/>
-      <c r="O19" s="121"/>
-      <c r="P19" s="121"/>
-      <c r="Q19" s="108"/>
-      <c r="R19" s="121"/>
-      <c r="S19" s="108"/>
-      <c r="T19" s="120"/>
-      <c r="U19" s="108"/>
-      <c r="V19" s="120"/>
-      <c r="W19" s="108"/>
+      <c r="D19" s="115"/>
+      <c r="E19" s="107"/>
+      <c r="F19" s="116"/>
+      <c r="G19" s="116"/>
+      <c r="H19" s="107"/>
+      <c r="I19" s="116"/>
+      <c r="J19" s="116"/>
+      <c r="K19" s="116"/>
+      <c r="L19" s="107"/>
+      <c r="M19" s="107"/>
+      <c r="N19" s="117"/>
+      <c r="O19" s="117"/>
+      <c r="P19" s="117"/>
+      <c r="Q19" s="107"/>
+      <c r="R19" s="117"/>
+      <c r="S19" s="107"/>
+      <c r="T19" s="116"/>
+      <c r="U19" s="107"/>
+      <c r="V19" s="116"/>
+      <c r="W19" s="107"/>
     </row>
     <row r="20" spans="1:23" ht="54.75" customHeight="1">
       <c r="A20" s="6"/>
       <c r="B20" s="6"/>
-      <c r="C20" s="166"/>
-      <c r="D20" s="166"/>
+      <c r="C20" s="162"/>
+      <c r="D20" s="162"/>
       <c r="E20" s="35"/>
       <c r="F20" s="36"/>
       <c r="G20" s="36"/>
@@ -2638,8 +2596,8 @@
     <row r="21" spans="1:23" ht="109.5" customHeight="1">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="167"/>
-      <c r="D21" s="167"/>
+      <c r="C21" s="163"/>
+      <c r="D21" s="163"/>
       <c r="E21" s="34"/>
       <c r="F21" s="49"/>
       <c r="G21" s="49"/>
@@ -2647,24 +2605,24 @@
       <c r="I21" s="50"/>
       <c r="J21" s="34"/>
       <c r="K21" s="34"/>
-      <c r="L21" s="120"/>
-      <c r="M21" s="122"/>
-      <c r="N21" s="122"/>
-      <c r="O21" s="123"/>
-      <c r="P21" s="123"/>
-      <c r="Q21" s="122"/>
-      <c r="R21" s="122"/>
-      <c r="S21" s="113"/>
-      <c r="T21" s="113"/>
-      <c r="U21" s="113"/>
-      <c r="V21" s="113"/>
-      <c r="W21" s="120"/>
+      <c r="L21" s="116"/>
+      <c r="M21" s="118"/>
+      <c r="N21" s="107"/>
+      <c r="O21" s="116"/>
+      <c r="P21" s="116"/>
+      <c r="Q21" s="107"/>
+      <c r="R21" s="107"/>
+      <c r="S21" s="104"/>
+      <c r="T21" s="104"/>
+      <c r="U21" s="104"/>
+      <c r="V21" s="104"/>
+      <c r="W21" s="116"/>
     </row>
     <row r="22" spans="1:23" ht="123" customHeight="1">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="168"/>
-      <c r="D22" s="169"/>
+      <c r="C22" s="164"/>
+      <c r="D22" s="165"/>
       <c r="E22" s="34"/>
       <c r="F22" s="49"/>
       <c r="G22" s="49"/>
@@ -2672,18 +2630,18 @@
       <c r="I22" s="50"/>
       <c r="J22" s="34"/>
       <c r="K22" s="34"/>
-      <c r="L22" s="120"/>
-      <c r="M22" s="114"/>
-      <c r="N22" s="114"/>
-      <c r="O22" s="123"/>
-      <c r="P22" s="123"/>
-      <c r="Q22" s="122"/>
-      <c r="R22" s="122"/>
-      <c r="S22" s="114"/>
-      <c r="T22" s="114"/>
-      <c r="U22" s="114"/>
-      <c r="V22" s="114"/>
-      <c r="W22" s="120"/>
+      <c r="L22" s="116"/>
+      <c r="M22" s="110"/>
+      <c r="N22" s="111"/>
+      <c r="O22" s="116"/>
+      <c r="P22" s="116"/>
+      <c r="Q22" s="107"/>
+      <c r="R22" s="107"/>
+      <c r="S22" s="111"/>
+      <c r="T22" s="111"/>
+      <c r="U22" s="111"/>
+      <c r="V22" s="111"/>
+      <c r="W22" s="116"/>
     </row>
     <row r="23" spans="1:23" s="39" customFormat="1" ht="16.5" customHeight="1">
       <c r="D23" s="40"/>
@@ -2710,10 +2668,10 @@
     <row r="24" spans="1:23" s="11" customFormat="1" ht="77.25" thickBot="1">
       <c r="A24" s="8"/>
       <c r="B24" s="8"/>
-      <c r="C24" s="164" t="s">
+      <c r="C24" s="160" t="s">
         <v>83</v>
       </c>
-      <c r="D24" s="165"/>
+      <c r="D24" s="161"/>
       <c r="E24" s="60" t="s">
         <v>88</v>
       </c>
@@ -2729,98 +2687,98 @@
       <c r="I24" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="J24" s="152" t="s">
+      <c r="J24" s="142" t="s">
         <v>50</v>
       </c>
-      <c r="K24" s="152"/>
+      <c r="K24" s="142"/>
       <c r="L24" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="M24" s="152" t="s">
+      <c r="M24" s="142" t="s">
         <v>52</v>
       </c>
-      <c r="N24" s="152"/>
-      <c r="O24" s="152"/>
-      <c r="P24" s="152"/>
-      <c r="Q24" s="152" t="s">
+      <c r="N24" s="142"/>
+      <c r="O24" s="142"/>
+      <c r="P24" s="142"/>
+      <c r="Q24" s="142" t="s">
         <v>53</v>
       </c>
-      <c r="R24" s="152"/>
-      <c r="S24" s="152" t="s">
+      <c r="R24" s="142"/>
+      <c r="S24" s="142" t="s">
         <v>54</v>
       </c>
-      <c r="T24" s="152"/>
-      <c r="U24" s="152" t="s">
+      <c r="T24" s="142"/>
+      <c r="U24" s="142" t="s">
         <v>55</v>
       </c>
-      <c r="V24" s="152"/>
+      <c r="V24" s="142"/>
       <c r="W24" s="9" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:23" s="11" customFormat="1" ht="112.5" customHeight="1" thickBot="1">
-      <c r="A25" s="91" t="s">
+      <c r="A25" s="90" t="s">
         <v>5</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="124"/>
-      <c r="E25" s="125"/>
-      <c r="F25" s="110"/>
-      <c r="G25" s="110"/>
-      <c r="H25" s="110"/>
-      <c r="I25" s="110"/>
-      <c r="J25" s="126"/>
-      <c r="K25" s="127"/>
-      <c r="L25" s="110"/>
-      <c r="M25" s="110"/>
-      <c r="N25" s="127"/>
-      <c r="O25" s="127"/>
-      <c r="P25" s="127"/>
-      <c r="Q25" s="110"/>
-      <c r="R25" s="128"/>
-      <c r="S25" s="110"/>
-      <c r="T25" s="127"/>
-      <c r="U25" s="110"/>
-      <c r="V25" s="127"/>
-      <c r="W25" s="110"/>
+      <c r="D25" s="119"/>
+      <c r="E25" s="132"/>
+      <c r="F25" s="104"/>
+      <c r="G25" s="104"/>
+      <c r="H25" s="104"/>
+      <c r="I25" s="104"/>
+      <c r="J25" s="105"/>
+      <c r="K25" s="131"/>
+      <c r="L25" s="104"/>
+      <c r="M25" s="104"/>
+      <c r="N25" s="131"/>
+      <c r="O25" s="131"/>
+      <c r="P25" s="131"/>
+      <c r="Q25" s="104"/>
+      <c r="R25" s="122"/>
+      <c r="S25" s="104"/>
+      <c r="T25" s="131"/>
+      <c r="U25" s="104"/>
+      <c r="V25" s="131"/>
+      <c r="W25" s="104"/>
     </row>
     <row r="26" spans="1:23" s="11" customFormat="1" ht="114" customHeight="1" thickBot="1">
-      <c r="A26" s="92" t="s">
+      <c r="A26" s="91" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="119"/>
-      <c r="E26" s="129"/>
-      <c r="F26" s="111"/>
-      <c r="G26" s="111"/>
-      <c r="H26" s="111"/>
-      <c r="I26" s="111"/>
-      <c r="J26" s="111"/>
-      <c r="K26" s="127"/>
-      <c r="L26" s="111"/>
-      <c r="M26" s="111"/>
-      <c r="N26" s="127"/>
-      <c r="O26" s="127"/>
-      <c r="P26" s="127"/>
-      <c r="Q26" s="111"/>
-      <c r="R26" s="130"/>
-      <c r="S26" s="111"/>
-      <c r="T26" s="127"/>
-      <c r="U26" s="111"/>
-      <c r="V26" s="127"/>
-      <c r="W26" s="111"/>
+      <c r="D26" s="115"/>
+      <c r="E26" s="133"/>
+      <c r="F26" s="107"/>
+      <c r="G26" s="107"/>
+      <c r="H26" s="107"/>
+      <c r="I26" s="107"/>
+      <c r="J26" s="107"/>
+      <c r="K26" s="131"/>
+      <c r="L26" s="107"/>
+      <c r="M26" s="107"/>
+      <c r="N26" s="131"/>
+      <c r="O26" s="131"/>
+      <c r="P26" s="131"/>
+      <c r="Q26" s="107"/>
+      <c r="R26" s="120"/>
+      <c r="S26" s="107"/>
+      <c r="T26" s="131"/>
+      <c r="U26" s="107"/>
+      <c r="V26" s="131"/>
+      <c r="W26" s="107"/>
     </row>
     <row r="27" spans="1:23" s="11" customFormat="1" ht="39" thickBot="1">
       <c r="A27" s="8"/>
       <c r="B27" s="8"/>
-      <c r="C27" s="155"/>
-      <c r="D27" s="156"/>
+      <c r="C27" s="143"/>
+      <c r="D27" s="144"/>
       <c r="E27" s="68"/>
       <c r="F27" s="68"/>
       <c r="G27" s="68"/>
@@ -2868,8 +2826,8 @@
     <row r="28" spans="1:23" s="11" customFormat="1" ht="79.5" customHeight="1">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
-      <c r="C28" s="161"/>
-      <c r="D28" s="162"/>
+      <c r="C28" s="157"/>
+      <c r="D28" s="158"/>
       <c r="E28" s="74"/>
       <c r="F28" s="74"/>
       <c r="G28" s="74"/>
@@ -2878,23 +2836,23 @@
       <c r="J28" s="75"/>
       <c r="K28" s="75"/>
       <c r="L28" s="74"/>
-      <c r="M28" s="131"/>
-      <c r="N28" s="131"/>
-      <c r="O28" s="131"/>
-      <c r="P28" s="131"/>
-      <c r="Q28" s="131"/>
-      <c r="R28" s="131"/>
-      <c r="S28" s="131"/>
-      <c r="T28" s="131"/>
-      <c r="U28" s="131"/>
-      <c r="V28" s="131"/>
+      <c r="M28" s="121"/>
+      <c r="N28" s="121"/>
+      <c r="O28" s="121"/>
+      <c r="P28" s="121"/>
+      <c r="Q28" s="121"/>
+      <c r="R28" s="121"/>
+      <c r="S28" s="121"/>
+      <c r="T28" s="121"/>
+      <c r="U28" s="121"/>
+      <c r="V28" s="121"/>
       <c r="W28" s="54"/>
     </row>
     <row r="29" spans="1:23" s="11" customFormat="1" ht="103.5" customHeight="1">
-      <c r="A29" s="100"/>
-      <c r="B29" s="100"/>
-      <c r="C29" s="163"/>
-      <c r="D29" s="163"/>
+      <c r="A29" s="99"/>
+      <c r="B29" s="99"/>
+      <c r="C29" s="159"/>
+      <c r="D29" s="159"/>
       <c r="E29" s="70"/>
       <c r="F29" s="70"/>
       <c r="G29" s="70"/>
@@ -2903,16 +2861,16 @@
       <c r="J29" s="67"/>
       <c r="K29" s="67"/>
       <c r="L29" s="70"/>
-      <c r="M29" s="115"/>
-      <c r="N29" s="115"/>
-      <c r="O29" s="115"/>
-      <c r="P29" s="115"/>
-      <c r="Q29" s="115"/>
-      <c r="R29" s="115"/>
-      <c r="S29" s="115"/>
-      <c r="T29" s="115"/>
-      <c r="U29" s="115"/>
-      <c r="V29" s="115"/>
+      <c r="M29" s="111"/>
+      <c r="N29" s="111"/>
+      <c r="O29" s="111"/>
+      <c r="P29" s="111"/>
+      <c r="Q29" s="111"/>
+      <c r="R29" s="111"/>
+      <c r="S29" s="111"/>
+      <c r="T29" s="111"/>
+      <c r="U29" s="111"/>
+      <c r="V29" s="111"/>
       <c r="W29" s="54"/>
     </row>
     <row r="30" spans="1:23" s="76" customFormat="1">
@@ -2940,10 +2898,10 @@
     <row r="31" spans="1:23" s="11" customFormat="1" ht="76.5">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
-      <c r="C31" s="178" t="s">
+      <c r="C31" s="155" t="s">
         <v>84</v>
       </c>
-      <c r="D31" s="178"/>
+      <c r="D31" s="155"/>
       <c r="E31" s="60" t="s">
         <v>61</v>
       </c>
@@ -2956,101 +2914,101 @@
       <c r="H31" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="I31" s="67" t="s">
+      <c r="I31" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="J31" s="179" t="s">
+      <c r="J31" s="156" t="s">
         <v>66</v>
       </c>
-      <c r="K31" s="179"/>
+      <c r="K31" s="156"/>
       <c r="L31" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="M31" s="152" t="s">
+      <c r="M31" s="142" t="s">
         <v>89</v>
       </c>
-      <c r="N31" s="152"/>
-      <c r="O31" s="152"/>
-      <c r="P31" s="152"/>
-      <c r="Q31" s="152" t="s">
+      <c r="N31" s="142"/>
+      <c r="O31" s="142"/>
+      <c r="P31" s="142"/>
+      <c r="Q31" s="142" t="s">
         <v>68</v>
       </c>
-      <c r="R31" s="152"/>
-      <c r="S31" s="152" t="s">
+      <c r="R31" s="142"/>
+      <c r="S31" s="142" t="s">
         <v>69</v>
       </c>
-      <c r="T31" s="152"/>
-      <c r="U31" s="152" t="s">
+      <c r="T31" s="142"/>
+      <c r="U31" s="142" t="s">
         <v>70</v>
       </c>
-      <c r="V31" s="152"/>
+      <c r="V31" s="142"/>
       <c r="W31" s="9" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:23" s="11" customFormat="1" ht="112.5" customHeight="1" thickBot="1">
-      <c r="A32" s="89" t="s">
+      <c r="A32" s="88" t="s">
         <v>5</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="116"/>
-      <c r="E32" s="132"/>
-      <c r="F32" s="133"/>
-      <c r="G32" s="133"/>
-      <c r="H32" s="133"/>
-      <c r="I32" s="134"/>
+      <c r="D32" s="112"/>
+      <c r="E32" s="134"/>
+      <c r="F32" s="135"/>
+      <c r="G32" s="135"/>
+      <c r="H32" s="135"/>
+      <c r="I32" s="135"/>
       <c r="J32" s="135"/>
-      <c r="K32" s="136"/>
-      <c r="L32" s="133"/>
-      <c r="M32" s="133"/>
-      <c r="N32" s="136"/>
-      <c r="O32" s="136"/>
-      <c r="P32" s="136"/>
-      <c r="Q32" s="133"/>
-      <c r="R32" s="137"/>
-      <c r="S32" s="133"/>
-      <c r="T32" s="136"/>
-      <c r="U32" s="133"/>
-      <c r="V32" s="136"/>
-      <c r="W32" s="110"/>
+      <c r="K32" s="122"/>
+      <c r="L32" s="135"/>
+      <c r="M32" s="135"/>
+      <c r="N32" s="122"/>
+      <c r="O32" s="122"/>
+      <c r="P32" s="122"/>
+      <c r="Q32" s="135"/>
+      <c r="R32" s="122"/>
+      <c r="S32" s="135"/>
+      <c r="T32" s="122"/>
+      <c r="U32" s="135"/>
+      <c r="V32" s="122"/>
+      <c r="W32" s="104"/>
     </row>
     <row r="33" spans="1:23" s="11" customFormat="1" ht="114" customHeight="1" thickBot="1">
-      <c r="A33" s="90" t="s">
+      <c r="A33" s="89" t="s">
         <v>4</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="D33" s="119"/>
-      <c r="E33" s="129"/>
-      <c r="F33" s="111"/>
-      <c r="G33" s="111"/>
-      <c r="H33" s="111"/>
-      <c r="I33" s="138"/>
-      <c r="J33" s="138"/>
-      <c r="K33" s="127"/>
-      <c r="L33" s="111"/>
-      <c r="M33" s="111"/>
-      <c r="N33" s="127"/>
-      <c r="O33" s="127"/>
-      <c r="P33" s="127"/>
-      <c r="Q33" s="111"/>
-      <c r="R33" s="130"/>
-      <c r="S33" s="111"/>
-      <c r="T33" s="127"/>
-      <c r="U33" s="111"/>
-      <c r="V33" s="127"/>
-      <c r="W33" s="111"/>
+      <c r="D33" s="115"/>
+      <c r="E33" s="133"/>
+      <c r="F33" s="107"/>
+      <c r="G33" s="107"/>
+      <c r="H33" s="107"/>
+      <c r="I33" s="107"/>
+      <c r="J33" s="107"/>
+      <c r="K33" s="120"/>
+      <c r="L33" s="107"/>
+      <c r="M33" s="107"/>
+      <c r="N33" s="120"/>
+      <c r="O33" s="120"/>
+      <c r="P33" s="120"/>
+      <c r="Q33" s="107"/>
+      <c r="R33" s="120"/>
+      <c r="S33" s="107"/>
+      <c r="T33" s="120"/>
+      <c r="U33" s="107"/>
+      <c r="V33" s="120"/>
+      <c r="W33" s="107"/>
     </row>
     <row r="34" spans="1:23" s="11" customFormat="1" ht="39" thickBot="1">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
-      <c r="C34" s="155"/>
-      <c r="D34" s="156"/>
+      <c r="C34" s="143"/>
+      <c r="D34" s="144"/>
       <c r="E34" s="68"/>
       <c r="F34" s="68"/>
       <c r="G34" s="68"/>
@@ -3069,10 +3027,10 @@
       <c r="N34" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="O34" s="79" t="s">
+      <c r="O34" s="136" t="s">
         <v>73</v>
       </c>
-      <c r="P34" s="79" t="s">
+      <c r="P34" s="136" t="s">
         <v>74</v>
       </c>
       <c r="Q34" s="59" t="s">
@@ -3098,51 +3056,51 @@
     <row r="35" spans="1:23" s="11" customFormat="1" ht="93.75" customHeight="1">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
-      <c r="C35" s="182"/>
-      <c r="D35" s="183"/>
-      <c r="E35" s="139"/>
-      <c r="F35" s="139"/>
-      <c r="G35" s="139"/>
-      <c r="H35" s="139"/>
-      <c r="I35" s="139"/>
-      <c r="J35" s="141"/>
-      <c r="K35" s="141"/>
-      <c r="L35" s="139"/>
-      <c r="M35" s="113"/>
-      <c r="N35" s="113"/>
-      <c r="O35" s="140"/>
-      <c r="P35" s="140"/>
-      <c r="Q35" s="113"/>
-      <c r="R35" s="113"/>
-      <c r="S35" s="113"/>
-      <c r="T35" s="113"/>
-      <c r="U35" s="113"/>
-      <c r="V35" s="113"/>
+      <c r="C35" s="145"/>
+      <c r="D35" s="146"/>
+      <c r="E35" s="123"/>
+      <c r="F35" s="123"/>
+      <c r="G35" s="123"/>
+      <c r="H35" s="123"/>
+      <c r="I35" s="123"/>
+      <c r="J35" s="124"/>
+      <c r="K35" s="124"/>
+      <c r="L35" s="123"/>
+      <c r="M35" s="104"/>
+      <c r="N35" s="104"/>
+      <c r="O35" s="104"/>
+      <c r="P35" s="104"/>
+      <c r="Q35" s="104"/>
+      <c r="R35" s="104"/>
+      <c r="S35" s="104"/>
+      <c r="T35" s="104"/>
+      <c r="U35" s="104"/>
+      <c r="V35" s="104"/>
       <c r="W35" s="54"/>
     </row>
     <row r="36" spans="1:23" s="11" customFormat="1" ht="99" customHeight="1">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
-      <c r="C36" s="182"/>
-      <c r="D36" s="183"/>
-      <c r="E36" s="139"/>
-      <c r="F36" s="139"/>
-      <c r="G36" s="139"/>
-      <c r="H36" s="139"/>
-      <c r="I36" s="139"/>
-      <c r="J36" s="141"/>
-      <c r="K36" s="141"/>
-      <c r="L36" s="139"/>
-      <c r="M36" s="114"/>
-      <c r="N36" s="114"/>
-      <c r="O36" s="140"/>
-      <c r="P36" s="140"/>
-      <c r="Q36" s="114"/>
-      <c r="R36" s="114"/>
-      <c r="S36" s="114"/>
-      <c r="T36" s="114"/>
-      <c r="U36" s="114"/>
-      <c r="V36" s="114"/>
+      <c r="C36" s="145"/>
+      <c r="D36" s="146"/>
+      <c r="E36" s="123"/>
+      <c r="F36" s="123"/>
+      <c r="G36" s="123"/>
+      <c r="H36" s="123"/>
+      <c r="I36" s="123"/>
+      <c r="J36" s="124"/>
+      <c r="K36" s="124"/>
+      <c r="L36" s="123"/>
+      <c r="M36" s="111"/>
+      <c r="N36" s="111"/>
+      <c r="O36" s="111"/>
+      <c r="P36" s="111"/>
+      <c r="Q36" s="111"/>
+      <c r="R36" s="111"/>
+      <c r="S36" s="111"/>
+      <c r="T36" s="111"/>
+      <c r="U36" s="111"/>
+      <c r="V36" s="111"/>
       <c r="W36" s="54"/>
     </row>
     <row r="37" spans="1:23" s="11" customFormat="1">
@@ -3175,139 +3133,107 @@
       <c r="C38" s="19"/>
     </row>
     <row r="39" spans="1:23" s="13" customFormat="1" ht="90.75" thickBot="1">
-      <c r="A39" s="97" t="s">
+      <c r="A39" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="94"/>
-      <c r="C39" s="184" t="s">
+      <c r="B39" s="93"/>
+      <c r="C39" s="147" t="s">
         <v>90</v>
       </c>
-      <c r="D39" s="185"/>
-      <c r="E39" s="83" t="s">
+      <c r="D39" s="148"/>
+      <c r="E39" s="82" t="s">
         <v>107</v>
       </c>
-      <c r="F39" s="84" t="s">
+      <c r="F39" s="83" t="s">
         <v>108</v>
       </c>
-      <c r="G39" s="84" t="s">
+      <c r="G39" s="83" t="s">
         <v>109</v>
       </c>
-      <c r="H39" s="85" t="s">
+      <c r="H39" s="84" t="s">
         <v>91</v>
       </c>
-      <c r="I39" s="86" t="s">
+      <c r="I39" s="85" t="s">
         <v>92</v>
       </c>
-      <c r="J39" s="80"/>
-      <c r="K39" s="80"/>
-      <c r="L39" s="80"/>
+      <c r="J39" s="79"/>
+      <c r="K39" s="79"/>
+      <c r="L39" s="79"/>
       <c r="M39" s="20"/>
     </row>
     <row r="40" spans="1:23" ht="140.25" customHeight="1">
-      <c r="A40" s="95" t="s">
+      <c r="A40" s="94" t="s">
         <v>5</v>
       </c>
       <c r="B40" s="6"/>
-      <c r="C40" s="176"/>
-      <c r="D40" s="177"/>
-      <c r="E40" s="142"/>
-      <c r="F40" s="142"/>
-      <c r="G40" s="142"/>
-      <c r="H40" s="143"/>
-      <c r="I40" s="144"/>
+      <c r="C40" s="140"/>
+      <c r="D40" s="139"/>
+      <c r="E40" s="137"/>
+      <c r="F40" s="137"/>
+      <c r="G40" s="137"/>
+      <c r="H40" s="125"/>
+      <c r="I40" s="126"/>
       <c r="K40" s="78"/>
     </row>
     <row r="41" spans="1:23" ht="140.25" customHeight="1">
-      <c r="A41" s="96" t="s">
+      <c r="A41" s="95" t="s">
         <v>4</v>
       </c>
       <c r="B41" s="6"/>
-      <c r="C41" s="180"/>
-      <c r="D41" s="181"/>
-      <c r="E41" s="145"/>
-      <c r="F41" s="145"/>
-      <c r="G41" s="145"/>
-      <c r="H41" s="108"/>
-      <c r="I41" s="146"/>
+      <c r="C41" s="141"/>
+      <c r="D41" s="138"/>
+      <c r="E41" s="138"/>
+      <c r="F41" s="138"/>
+      <c r="G41" s="138"/>
+      <c r="H41" s="107"/>
+      <c r="I41" s="127"/>
       <c r="K41" s="78"/>
     </row>
     <row r="42" spans="1:23" ht="78.75" customHeight="1">
-      <c r="A42" s="93"/>
+      <c r="A42" s="92"/>
       <c r="B42" s="6"/>
-      <c r="C42" s="170"/>
-      <c r="D42" s="171"/>
-      <c r="E42" s="81" t="s">
+      <c r="C42" s="149"/>
+      <c r="D42" s="150"/>
+      <c r="E42" s="80" t="s">
         <v>97</v>
       </c>
-      <c r="F42" s="81" t="s">
+      <c r="F42" s="80" t="s">
         <v>96</v>
       </c>
-      <c r="G42" s="81" t="s">
+      <c r="G42" s="80" t="s">
         <v>95</v>
       </c>
-      <c r="H42" s="81" t="s">
+      <c r="H42" s="80" t="s">
         <v>93</v>
       </c>
-      <c r="I42" s="82" t="s">
+      <c r="I42" s="81" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:23" ht="102" customHeight="1">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
-      <c r="C43" s="172"/>
-      <c r="D43" s="173"/>
-      <c r="E43" s="105"/>
-      <c r="F43" s="105"/>
-      <c r="G43" s="105"/>
-      <c r="H43" s="105"/>
-      <c r="I43" s="147"/>
+      <c r="C43" s="151"/>
+      <c r="D43" s="152"/>
+      <c r="E43" s="104"/>
+      <c r="F43" s="104"/>
+      <c r="G43" s="104"/>
+      <c r="H43" s="104"/>
+      <c r="I43" s="128"/>
     </row>
     <row r="44" spans="1:23" ht="111.75" customHeight="1" thickBot="1">
       <c r="A44" s="6"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="174"/>
-      <c r="D44" s="175"/>
-      <c r="E44" s="148"/>
-      <c r="F44" s="148"/>
-      <c r="G44" s="148"/>
-      <c r="H44" s="148"/>
-      <c r="I44" s="149"/>
+      <c r="C44" s="153"/>
+      <c r="D44" s="154"/>
+      <c r="E44" s="129"/>
+      <c r="F44" s="129"/>
+      <c r="G44" s="129"/>
+      <c r="H44" s="129"/>
+      <c r="I44" s="130"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="U31:V31"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="S31:T31"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="M31:P31"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="M24:P24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="S24:T24"/>
-    <mergeCell ref="U24:V24"/>
+  <mergeCells count="39">
     <mergeCell ref="M17:P17"/>
     <mergeCell ref="Q17:R17"/>
     <mergeCell ref="S17:T17"/>
@@ -3317,6 +3243,36 @@
     <mergeCell ref="Q10:R10"/>
     <mergeCell ref="S10:T10"/>
     <mergeCell ref="U10:V10"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="M24:P24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="S24:T24"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="S31:T31"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="M31:P31"/>
+    <mergeCell ref="U31:V31"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C39:D39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>